<commit_message>
Fixing call to build array predictions.
</commit_message>
<xml_diff>
--- a/test/resources/RemixDataBuilder.xlsx
+++ b/test/resources/RemixDataBuilder.xlsx
@@ -48,19 +48,19 @@
     <t>Create Contest Definition</t>
   </si>
   <si>
-    <t>Rusia2018Test11</t>
-  </si>
-  <si>
     <t>Create Contest Pool</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>GuillePool</t>
-  </si>
-  <si>
     <t>Amount Per Player</t>
+  </si>
+  <si>
+    <t>Russia2018</t>
+  </si>
+  <si>
+    <t>Bitbrackets</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -432,7 +432,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -458,15 +458,15 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1">
         <f>DATE(B5,C5,D5)</f>
-        <v>43252</v>
+        <v>43265</v>
       </c>
       <c r="F5" s="2">
         <f>(E5-DATE(1970,1,1))*86400</f>
-        <v>1527811200</v>
+        <v>1528934400</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -477,18 +477,18 @@
         <v>2018</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1">
         <f>DATE(B6,C6,D6)</f>
-        <v>43282</v>
+        <v>43280</v>
       </c>
       <c r="F6" s="2">
         <f>(E6-DATE(1970,1,1))*86400</f>
-        <v>1530403200</v>
+        <v>1530230400</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -553,20 +553,20 @@
       </c>
       <c r="B13" t="str">
         <f>CONCATENATE("""",B3,""",",C4, ",",F5, ",",F6, ",",G7, ",",C8, ",",B9, ",",B10)</f>
-        <v>"Rusia2018Test11",10000000000000000,1527811200,1530403200,345600,10000000000000000000,10,10</v>
+        <v>"Russia2018",10000000000000000,1528934400,1530230400,345600,10000000000000000000,10,10</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>0.01</v>
@@ -578,11 +578,11 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" t="str">
         <f>CONCATENATE("""",B15,""",""",B3,""",",C16)</f>
-        <v>"GuillePool","Rusia2018Test11",10000000000000000</v>
+        <v>"Bitbrackets","Russia2018",10000000000000000</v>
       </c>
       <c r="C18" t="str">
         <f>CONCATENATE("FEE:", C4)</f>

</xml_diff>